<commit_message>
Update ENTREGA 1 - Estatística.xlsx
</commit_message>
<xml_diff>
--- a/documentos/Entrega 1/Análise Descritiva de Dados/ENTREGA 1 - Estatística.xlsx
+++ b/documentos/Entrega 1/Análise Descritiva de Dados/ENTREGA 1 - Estatística.xlsx
@@ -1,78 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\24025899\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1E489E-7BAB-4814-8370-A7DA9E26526B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB3C378-654E-4AF3-9B92-32BB06BFD4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{BCAF05DD-5CE8-4CFA-A174-F682FC9CB0E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCAF05DD-5CE8-4CFA-A174-F682FC9CB0E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Entregas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Planilha1!$B$4:$B$8</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Planilha1!$A$17:$A$101</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Planilha1!$A$17:$A$101</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Entregas!$A$17:$A$101</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Entregas!$A$7:$A$11</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Entregas!$B$7:$B$11</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Entregas!$A$7:$A$11</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Entregas!$B$7:$B$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Entrega 1 - Análise Descritiva de Dados</t>
   </si>
   <si>
-    <t>Os dados apresentados a seguir foram retirados de uma pesquisa de mercado para melhor entendermos as necessidades dos usuários.</t>
-  </si>
-  <si>
-    <t>Aqui estão os dados dos motivos que as pessoas se sentem inseguras:</t>
-  </si>
-  <si>
-    <t>1 - Falta de identificação/verificação do motorista/passageiro</t>
-  </si>
-  <si>
-    <t>2 - Viagem por locais perigosos</t>
-  </si>
-  <si>
-    <t>4 - Comunicação limitada com contatos de emergência</t>
-  </si>
-  <si>
-    <t>3 - Falta de um botão de emergência acessível</t>
-  </si>
-  <si>
-    <t>5 - Outros</t>
-  </si>
-  <si>
-    <t>MÉDIA DAS RESPOSTAS:</t>
-  </si>
-  <si>
-    <t>TOTAL DE RESPOSTAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HISTOGRAMA: </t>
-  </si>
-  <si>
-    <t>95°PERCENTIL:</t>
+    <t xml:space="preserve">Os dados apresentados a seguir foram retirados de uma pesquisa realizada pelo Datafolha para o Observatório Nacional de Segurança Viária (ONSV) em abril de 2019 entrevistou 3.531 pessoas de todas as regiões do Brasil </t>
+  </si>
+  <si>
+    <t>Fonte: https://agenciabrasil.ebc.com.br/geral/noticia/2019-05/aumento-do-uso-de-aplicativos-reduz-mortes-no-transito-diz-pesquisa</t>
+  </si>
+  <si>
+    <t>Média Nacional</t>
+  </si>
+  <si>
+    <t>Região Metropolitana de São Paulo</t>
+  </si>
+  <si>
+    <t>Os dados a seguir mostram a porcentagem de pessoas que utilizam as viagens de aplicativos após beber, de diferentes locais e faixas etárias</t>
+  </si>
+  <si>
+    <t>Região Metropolitana do Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Jovens até 24 anos</t>
+  </si>
+  <si>
+    <t>Idosos (60 anos ou mais)</t>
+  </si>
+  <si>
+    <t>Total de respostas</t>
+  </si>
+  <si>
+    <t>Média geométrica(fator)</t>
+  </si>
+  <si>
+    <t>Média geométrica(%)</t>
+  </si>
+  <si>
+    <t>95ºPercentil(fator)</t>
+  </si>
+  <si>
+    <t>95ºPercentil(%)</t>
+  </si>
+  <si>
+    <t>Histograma:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +104,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,9 +139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,8 +167,11 @@
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -142,7 +179,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Motivos de insegurança em apps de mobilidade</cx:v>
+          <cx:v>Histograma</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -162,21 +199,21 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Motivos de insegurança em apps de mobilidade</a:t>
+            <a:t>Histograma</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{0D98E70D-940F-45A2-90D7-222021DF08B4}">
-          <cx:dataLabels>
+        <cx:series layoutId="clusteredColumn" uniqueId="{44E97CB6-D719-4CC0-BEA6-BEB4B1944E83}">
+          <cx:dataLabels pos="inEnd">
             <cx:visibility seriesName="0" categoryName="0" value="1"/>
           </cx:dataLabels>
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:binning intervalClosed="r">
-              <cx:binSize val="1"/>
+              <cx:binSize val="0.05000000000000001"/>
             </cx:binning>
           </cx:layoutPr>
         </cx:series>
@@ -186,7 +223,7 @@
         <cx:title>
           <cx:tx>
             <cx:txData>
-              <cx:v>Número de respostas</cx:v>
+              <cx:v>Pessoas que usam aplicativos de viagem após beberem(%)</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:txPr>
@@ -206,12 +243,11 @@
                   </a:solidFill>
                   <a:latin typeface="Calibri" panose="020F0502020204030204"/>
                 </a:rPr>
-                <a:t>Número de respostas</a:t>
+                <a:t>Pessoas que usam aplicativos de viagem após beberem(%)</a:t>
               </a:r>
             </a:p>
           </cx:txPr>
         </cx:title>
-        <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
@@ -219,7 +255,7 @@
         <cx:title>
           <cx:tx>
             <cx:txData>
-              <cx:v>Motivos(baseados na legenda}</cx:v>
+              <cx:v>Ocorrência de dados</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:txPr>
@@ -239,7 +275,7 @@
                   </a:solidFill>
                   <a:latin typeface="Calibri" panose="020F0502020204030204"/>
                 </a:rPr>
-                <a:t>Motivos(baseados na legenda}</a:t>
+                <a:t>Ocorrência de dados</a:t>
               </a:r>
             </a:p>
           </cx:txPr>
@@ -804,25 +840,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1732</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>50523</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>338570</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4622523</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>92765</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Gráfico 2">
+            <xdr:cNvPr id="2" name="Gráfico 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16A999C3-D0FC-428F-B00B-D11A34CE448F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7667DAF-0E34-F798-837B-45C1D36DDFE0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -849,8 +885,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8210550" y="2662237"/>
-              <a:ext cx="4579793" cy="2743200"/>
+              <a:off x="50523" y="3445565"/>
+              <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -884,9 +920,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -924,7 +960,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1030,7 +1066,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1172,7 +1208,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1180,15 +1216,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F285933C-D035-4E8B-913E-E8B6E8DC961C}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="123" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,511 +1242,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>27</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.68500000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="B10" s="2">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.59</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <f>SUM(B4:B8)</f>
-        <v>87</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <f>AVERAGE(B4:B8)</f>
-        <v>17.399999999999999</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3531</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
-        <f>_xlfn.PERCENTILE.INC(B4:B8,0.95)</f>
-        <v>26</v>
+        <f>GEOMEAN(B7:B11)</f>
+        <v>0.7166645427476751</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.71660000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <f>_xlfn.PERCENTILE.INC(B7:B11,0.95)</f>
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Correção da entrega 1 de estatistica
</commit_message>
<xml_diff>
--- a/documentos/Entrega 1/Análise Descritiva de Dados/ENTREGA 1 - Estatística.xlsx
+++ b/documentos/Entrega 1/Análise Descritiva de Dados/ENTREGA 1 - Estatística.xlsx
@@ -5,22 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\GitHub\Projeto6\documentos\Entrega 1\Análise Descritiva de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB3C378-654E-4AF3-9B92-32BB06BFD4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D2E766-D686-4956-A404-5808A6B37BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCAF05DD-5CE8-4CFA-A174-F682FC9CB0E1}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{BCAF05DD-5CE8-4CFA-A174-F682FC9CB0E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Entregas!$A$17:$A$101</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Entregas!$A$7:$A$11</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Entregas!$B$7:$B$11</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Entregas!$A$7:$A$11</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Entregas!$B$7:$B$11</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Entregas!$A$7:$A$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Entregas!$B$7:$B$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -139,11 +136,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -168,10 +164,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1218,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F285933C-D035-4E8B-913E-E8B6E8DC961C}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1268,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2">
@@ -1280,7 +1276,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2">
@@ -1294,7 +1290,7 @@
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>3531</v>
       </c>
     </row>
@@ -1338,7 +1334,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>